<commit_message>
Java Slide for List is done
Java Slide for List is done
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/CourseMaterials/Java/JavaCourse-Status.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/CourseMaterials/Java/JavaCourse-Status.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Teach_Tech@anodiam\IT\CourseMaterials\Java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3BB3C8D-C8EF-4CB3-AE1E-71FACF575A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCACE900-E628-4E11-A5E6-B18DACB3A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -230,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -242,7 +242,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -531,7 +530,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,174 +555,172 @@
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="C3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>24</v>
+      <c r="C4" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>24</v>
+      <c r="C5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="8" t="s">
+      <c r="C6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="8" t="s">
+      <c r="C9" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="8" t="s">
+      <c r="C11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="12" t="s">
+      <c r="C12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Java programs checked in
Java programs checked in
</commit_message>
<xml_diff>
--- a/Offline/BusinessManagement/Teach_Tech@anodiam/IT/CourseMaterials/Java/JavaCourse-Status.xlsx
+++ b/Offline/BusinessManagement/Teach_Tech@anodiam/IT/CourseMaterials/Java/JavaCourse-Status.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Anodiam\Docs\Offline\BusinessManagement\Teach_Tech@anodiam\IT\CourseMaterials\Java\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCACE900-E628-4E11-A5E6-B18DACB3A674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19440" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Java</t>
   </si>
@@ -112,9 +106,6 @@
   </si>
   <si>
     <t>Not Required</t>
-  </si>
-  <si>
-    <t>In Progress</t>
   </si>
   <si>
     <t>Collections</t>
@@ -123,8 +114,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,7 +139,7 @@
       <name val="Oxygen"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,12 +149,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -230,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -242,11 +227,10 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,28 +503,28 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -552,109 +536,109 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C3" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C5" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>24</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C8" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>14</v>
       </c>
@@ -664,39 +648,39 @@
       <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D10" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>18</v>
       </c>
@@ -706,21 +690,21 @@
       <c r="C13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>20</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>